<commit_message>
Add Rev D PCBA files
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0F929FC-04F4-43B1-9B57-8F4F40E513E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49402DEE-F3AC-45ED-9F8E-76DB197EF770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="570" windowWidth="19602" windowHeight="12348" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="6" yWindow="6" windowWidth="23028" windowHeight="13668" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
+    <sheet name="AD8314 Input Match" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="C_bp_lf">Sheet1!$B$13</definedName>
-    <definedName name="C_bp_lf_bot">Sheet1!$B$14</definedName>
-    <definedName name="C_bp_lf_top">Sheet1!$B$15</definedName>
-    <definedName name="f_r_bp_center">Sheet1!$B$7</definedName>
-    <definedName name="f_r_bp_lf">Sheet1!$B$10</definedName>
-    <definedName name="L_bp_hf">Sheet1!$B$23</definedName>
-    <definedName name="L_bp_lf">Sheet1!$B$12</definedName>
-    <definedName name="R_bp_L">Sheet1!$B$4</definedName>
-    <definedName name="R_s">Sheet1!$B$3</definedName>
-    <definedName name="w_r_bp_center">Sheet1!$B$8</definedName>
-    <definedName name="w_r_bp_lf">Sheet1!$B$11</definedName>
-    <definedName name="X_bp_L">Sheet1!$B$5</definedName>
-    <definedName name="Z_bp_L">Sheet1!$B$6</definedName>
+    <definedName name="C_bp_lf">'AD8314 Input Match'!$B$13</definedName>
+    <definedName name="C_bp_lf_bot">'AD8314 Input Match'!$B$14</definedName>
+    <definedName name="C_bp_lf_top">'AD8314 Input Match'!$B$15</definedName>
+    <definedName name="f_r_bp_center">'AD8314 Input Match'!$B$7</definedName>
+    <definedName name="f_r_bp_lf">'AD8314 Input Match'!$B$10</definedName>
+    <definedName name="L_bp_hf">'AD8314 Input Match'!$B$23</definedName>
+    <definedName name="L_bp_lf">'AD8314 Input Match'!$B$12</definedName>
+    <definedName name="R_bp_L">'AD8314 Input Match'!$B$4</definedName>
+    <definedName name="R_s">'AD8314 Input Match'!$B$3</definedName>
+    <definedName name="w_r_bp_center">'AD8314 Input Match'!$B$8</definedName>
+    <definedName name="w_r_bp_lf">'AD8314 Input Match'!$B$11</definedName>
+    <definedName name="X_bp_L">'AD8314 Input Match'!$B$5</definedName>
+    <definedName name="Z_bp_L">'AD8314 Input Match'!$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Parameter</t>
   </si>
@@ -178,6 +179,9 @@
   </si>
   <si>
     <t>R_bp,lf,tot</t>
+  </si>
+  <si>
+    <t>Noise figure calculation paper: https://www.ti.com/lit/an/slyt094/slyt094.pdf</t>
   </si>
 </sst>
 </file>
@@ -235,57 +239,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -654,11 +623,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1A8BE-3B15-4627-BC31-B7CF5AD21860}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="24.47265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F394AD-DB26-46BE-8BA2-682774885DB9}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
@@ -668,7 +674,7 @@
   <cols>
     <col min="1" max="1" width="26.3125" customWidth="1"/>
     <col min="2" max="2" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.89453125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="72.89453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -681,7 +687,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -700,7 +706,7 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -714,7 +720,7 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -728,7 +734,7 @@
       <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -743,7 +749,7 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -808,7 +814,7 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -828,13 +834,13 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -849,7 +855,7 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -857,88 +863,86 @@
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="4" t="s">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <f>R_s*(1+C_bp_lf_bot/C_bp_lf_top)^2</f>
         <v>2013.4128500415541</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <f>-1/(w_r_bp_center*1000000*C_bp_lf*0.000000000001)</f>
         <v>-45.298019211141273</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <f>1/(1/B18+1/X_bp_L)</f>
         <v>-31.735974214442297</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="4" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <f>1/(1/B17+1/B4)</f>
         <v>551.73674053203229</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="4" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <f>ABS(B20/B19)</f>
         <v>17.385215175809851</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22">
         <f>C_bp_lf/B21</f>
         <v>0.18541051140144393</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LTSpice work on tracking comparator
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49402DEE-F3AC-45ED-9F8E-76DB197EF770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C6ECB-64CB-4E97-9C6B-47CB4513D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6" yWindow="6" windowWidth="23028" windowHeight="13668" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="-78" yWindow="0" windowWidth="6474" windowHeight="13758" firstSheet="1" activeTab="2" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
     <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
     <sheet name="AD8314 Input Match" sheetId="1" r:id="rId2"/>
+    <sheet name="RP2040 PIO Delay Conversion" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="C_bp_lf">'AD8314 Input Match'!$B$13</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Parameter</t>
   </si>
@@ -182,6 +183,30 @@
   </si>
   <si>
     <t>Noise figure calculation paper: https://www.ti.com/lit/an/slyt094/slyt094.pdf</t>
+  </si>
+  <si>
+    <t>cycles</t>
+  </si>
+  <si>
+    <t>Post-Instruction Delay @ 16MHz</t>
+  </si>
+  <si>
+    <t>Post-Instruction Delay @ 48MHz</t>
+  </si>
+  <si>
+    <t>Total Time @ 16 Mhz</t>
+  </si>
+  <si>
+    <t>Total Cycles @ 16 MHz</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>Total Cycles @ 48 MHz</t>
+  </si>
+  <si>
+    <t>Instructions in Segment</t>
   </si>
 </sst>
 </file>
@@ -213,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +248,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -250,6 +281,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1A8BE-3B15-4627-BC31-B7CF5AD21860}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -664,7 +696,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
@@ -967,4 +999,97 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E2DF10-CE9B-482B-AF8C-BE5D5FAD84AE}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="31.62890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1">
+        <f>B2+B3</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/16</f>
+        <v>0.125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B5*48</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="6">
+        <f>B6-1</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update flash map for combined image
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\ads-bee\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jmcnelly\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C6ECB-64CB-4E97-9C6B-47CB4513D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFA3ACD-FE5B-466F-B0B9-CCA65F819041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="6474" windowHeight="13758" firstSheet="1" activeTab="2" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="1" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
     <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
     <sheet name="AD8314 Input Match" sheetId="1" r:id="rId2"/>
     <sheet name="RP2040 PIO Delay Conversion" sheetId="3" r:id="rId3"/>
+    <sheet name="EP2040 Memory Map" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="C_bp_lf">'AD8314 Input Match'!$B$13</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Parameter</t>
   </si>
@@ -207,6 +208,36 @@
   </si>
   <si>
     <t>Instructions in Segment</t>
+  </si>
+  <si>
+    <t>Start Address (Hex)</t>
+  </si>
+  <si>
+    <t>Size (kBytes)</t>
+  </si>
+  <si>
+    <t>0x</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>FLASH_BL</t>
+  </si>
+  <si>
+    <t>FLASH_APP0</t>
+  </si>
+  <si>
+    <t>FLASH_APP1</t>
+  </si>
+  <si>
+    <t>FLASH_HDR</t>
+  </si>
+  <si>
+    <t>Total Flash Size (kBytes)</t>
+  </si>
+  <si>
+    <t>Flash Utilized (kBytes)</t>
   </si>
 </sst>
 </file>
@@ -258,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -266,11 +297,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,6 +393,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E2DF10-CE9B-482B-AF8C-BE5D5FAD84AE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1092,4 +1239,118 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0193E163-E676-481D-8CE2-7F8B76453E50}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="13.20703125" customWidth="1"/>
+    <col min="4" max="4" width="15.20703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="9">
+        <v>10000000</v>
+      </c>
+      <c r="C4" s="15">
+        <v>180</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(B4)+C4*1000)</f>
+        <v>1002BF20</v>
+      </c>
+      <c r="C5" s="17">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="7" t="str">
+        <f t="shared" ref="B6:B7" si="0">DEC2HEX(HEX2DEC(B5)+C5*1000)</f>
+        <v>1002CEC0</v>
+      </c>
+      <c r="C6" s="17">
+        <f>(C1-(C4+C5))/2</f>
+        <v>8100</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>107E6760</v>
+      </c>
+      <c r="C7" s="19">
+        <f>C6</f>
+        <v>8100</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C4:C7)</f>
+        <v>16384</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change flash layout to use headers
* Change from appended CRC to separate header with app size and CRC.
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jmcnelly\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFA3ACD-FE5B-466F-B0B9-CCA65F819041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83DC6C3-4D37-4142-A0E4-E31906003A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="1" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Fix slow startup and post jump IRQ issues
* Disable interrupts and peripherals before boot jump to avoid unhandled IRQ crash.
* Alter settings constructor to avoid querying EEPROM before I2C is initialized (was causing 3 second startup delay).
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jmcnelly\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83DC6C3-4D37-4142-A0E4-E31906003A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA18C9E-3161-4D0D-94EE-4A0DF346522B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="1" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Parameter</t>
   </si>
@@ -231,13 +231,34 @@
     <t>FLASH_APP1</t>
   </si>
   <si>
-    <t>FLASH_HDR</t>
-  </si>
-  <si>
     <t>Total Flash Size (kBytes)</t>
   </si>
   <si>
     <t>Flash Utilized (kBytes)</t>
+  </si>
+  <si>
+    <t>FLASH_HDR0</t>
+  </si>
+  <si>
+    <t>FLASH_HDR1</t>
+  </si>
+  <si>
+    <t>Bootloader</t>
+  </si>
+  <si>
+    <t>Application 0 Header</t>
+  </si>
+  <si>
+    <t>Application 0 Data</t>
+  </si>
+  <si>
+    <t>Application 1 Header</t>
+  </si>
+  <si>
+    <t>Application 1 Data</t>
+  </si>
+  <si>
+    <t>10000000</t>
   </si>
 </sst>
 </file>
@@ -381,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,7 +414,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -404,20 +424,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -427,6 +440,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1243,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0193E163-E676-481D-8CE2-7F8B76453E50}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1256,93 +1276,125 @@
     <col min="4" max="4" width="15.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1">
         <v>16384</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="9">
-        <v>10000000</v>
-      </c>
-      <c r="C4" s="15">
-        <v>180</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="B4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="12">
+        <v>176</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="7" t="str">
-        <f>DEC2HEX(HEX2DEC(B4)+C4*1000)</f>
-        <v>1002BF20</v>
-      </c>
-      <c r="C5" s="17">
+      <c r="B5" s="18" t="str">
+        <f>DEC2HEX(HEX2DEC(B4)+C4*1024)</f>
+        <v>1002C000</v>
+      </c>
+      <c r="C5" s="19">
         <v>4</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="10" t="s">
+      <c r="D5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="7" t="str">
-        <f t="shared" ref="B6:B7" si="0">DEC2HEX(HEX2DEC(B5)+C5*1000)</f>
-        <v>1002CEC0</v>
-      </c>
-      <c r="C6" s="17">
-        <f>(C1-(C4+C5))/2</f>
+      <c r="B6" s="18" t="str">
+        <f t="shared" ref="B6:B8" si="0">DEC2HEX(HEX2DEC(B5)+C5*1024)</f>
+        <v>1002D000</v>
+      </c>
+      <c r="C6" s="19">
         <v>8100</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="11" t="s">
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="12" t="str">
+      <c r="B7" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>107E6760</v>
+        <v>10816000</v>
       </c>
       <c r="C7" s="19">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10817000</v>
+      </c>
+      <c r="C8" s="15">
         <f>C6</f>
         <v>8100</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D8" s="16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9">
-        <f>SUM(C4:C7)</f>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C4:C8)</f>
         <v>16384</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update firmware reference guide
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jmcnelly\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA18C9E-3161-4D0D-94EE-4A0DF346522B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F558213A-07A8-42B5-B5CF-948413342BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="1" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="-24160" yWindow="-5960" windowWidth="17280" windowHeight="9980" firstSheet="1" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
     <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
@@ -442,13 +442,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1285,10 +1285,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="11" t="s">
         <v>53</v>
       </c>
@@ -1320,11 +1320,11 @@
       <c r="A5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="18" t="str">
+      <c r="B5" t="str">
         <f>DEC2HEX(HEX2DEC(B4)+C4*1024)</f>
         <v>1002C000</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <v>4</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -1338,11 +1338,11 @@
       <c r="A6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="18" t="str">
+      <c r="B6" t="str">
         <f t="shared" ref="B6:B8" si="0">DEC2HEX(HEX2DEC(B5)+C5*1024)</f>
         <v>1002D000</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="17">
         <v>8100</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -1356,11 +1356,11 @@
       <c r="A7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="18" t="str">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>10816000</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="17">
         <v>4</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -1374,7 +1374,7 @@
       <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="18" t="str">
+      <c r="B8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>10817000</v>
       </c>

</xml_diff>

<commit_message>
Set up CPR filter test cases
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jmcnelly\git-checkouts\ads-bee\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F558213A-07A8-42B5-B5CF-948413342BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0655725A-656F-4D56-8FAC-A6D4B2723C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24160" yWindow="-5960" windowWidth="17280" windowHeight="9980" firstSheet="1" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="9984" firstSheet="3" activeTab="4" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
     <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
     <sheet name="AD8314 Input Match" sheetId="1" r:id="rId2"/>
     <sheet name="RP2040 PIO Delay Conversion" sheetId="3" r:id="rId3"/>
-    <sheet name="EP2040 Memory Map" sheetId="4" r:id="rId4"/>
+    <sheet name="RP2040 Memory Map" sheetId="4" r:id="rId4"/>
+    <sheet name="Mode S Beast RSSI Byte" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="C_bp_lf">'AD8314 Input Match'!$B$13</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
   <si>
     <t>Parameter</t>
   </si>
@@ -259,6 +260,30 @@
   </si>
   <si>
     <t>10000000</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>p_min</t>
+  </si>
+  <si>
+    <t>dBm</t>
+  </si>
+  <si>
+    <t>p_max</t>
+  </si>
+  <si>
+    <t>rssi_min</t>
+  </si>
+  <si>
+    <t>rssi_max</t>
+  </si>
+  <si>
+    <t>p_mid</t>
+  </si>
+  <si>
+    <t>rssi_mid</t>
   </si>
 </sst>
 </file>
@@ -445,10 +470,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0193E163-E676-481D-8CE2-7F8B76453E50}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1285,10 +1310,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="11" t="s">
         <v>53</v>
       </c>
@@ -1374,7 +1399,7 @@
       <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="19" t="str">
+      <c r="B8" s="18" t="str">
         <f t="shared" si="0"/>
         <v>10817000</v>
       </c>
@@ -1405,4 +1430,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74E8795-B0D8-4BFA-BD93-DE9627104852}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="25.734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>-95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3">
+        <v>-45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <f>255*10^((B2+45)/10)</f>
+        <v>2.5500000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
+        <f>255*10^((B3+45)/10)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <f>255*10^((B8+45)/10)</f>
+        <v>0.80638080334293594</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add more register reading for RX modem work
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jmcnelly\git-checkouts\ads-bee\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcnelly/git-checkouts/adsbee/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0655725A-656F-4D56-8FAC-A6D4B2723C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA26E33-C806-474F-9C24-897554662671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="9984" firstSheet="3" activeTab="4" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="4680" yWindow="1280" windowWidth="24760" windowHeight="17460" firstSheet="3" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
     <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
     <sheet name="AD8314 Input Match" sheetId="1" r:id="rId2"/>
     <sheet name="RP2040 PIO Delay Conversion" sheetId="3" r:id="rId3"/>
-    <sheet name="RP2040 Memory Map" sheetId="4" r:id="rId4"/>
-    <sheet name="Mode S Beast RSSI Byte" sheetId="5" r:id="rId5"/>
+    <sheet name="Si4362 Configuration" sheetId="6" r:id="rId4"/>
+    <sheet name="RP2040 Memory Map" sheetId="4" r:id="rId5"/>
+    <sheet name="Mode S Beast RSSI Byte" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="C_bp_lf">'AD8314 Input Match'!$B$13</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
   <si>
     <t>Parameter</t>
   </si>
@@ -284,6 +285,48 @@
   </si>
   <si>
     <t>rssi_mid</t>
+  </si>
+  <si>
+    <t>xosc_freq</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>ndec2</t>
+  </si>
+  <si>
+    <t>ndec1</t>
+  </si>
+  <si>
+    <t>ndec0</t>
+  </si>
+  <si>
+    <t>rxosr</t>
+  </si>
+  <si>
+    <t>dwn3byp</t>
+  </si>
+  <si>
+    <t>dwn2byp</t>
+  </si>
+  <si>
+    <t>sample_rate</t>
+  </si>
+  <si>
+    <t>Sample rate for receiver I/Q and Bit Clock Recovery (BCR).</t>
+  </si>
+  <si>
+    <t>kbps</t>
+  </si>
+  <si>
+    <t>rx_oversampling_rate</t>
+  </si>
+  <si>
+    <t>12 bits, indicates 8x the desired oversampling rate.</t>
+  </si>
+  <si>
+    <t>rx_bit_rate</t>
   </si>
 </sst>
 </file>
@@ -552,9 +595,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -592,7 +635,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -698,7 +741,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -840,7 +883,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,17 +897,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.47265625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -894,14 +937,14 @@
       <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.3125" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.89453125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -915,12 +958,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -934,7 +977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -948,7 +991,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -962,7 +1005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -977,7 +1020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -988,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1000,12 +1043,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1016,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1028,7 +1071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1042,7 +1085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1068,7 +1111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1083,13 +1126,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1104,7 +1147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1119,7 +1162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1131,7 +1174,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1143,7 +1186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1155,7 +1198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1170,7 +1213,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1201,12 +1244,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.62890625" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1231,7 +1274,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1239,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1251,7 +1294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1263,7 +1306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1272,7 +1315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1287,6 +1330,135 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C90358F-5FC6-0B4A-A773-03445C27E3CB}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>30000000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9">
+        <f>B2/B3/B4/B5/IF(B6,1,3)/IF(B7,1,2)/1000</f>
+        <v>250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12">
+        <f>B11/8</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14">
+        <f>B9/B12</f>
+        <v>166.66666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0193E163-E676-481D-8CE2-7F8B76453E50}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1294,14 +1466,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.26171875" customWidth="1"/>
-    <col min="3" max="3" width="13.20703125" customWidth="1"/>
-    <col min="4" max="4" width="15.20703125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>59</v>
       </c>
@@ -1309,7 +1481,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>52</v>
       </c>
@@ -1324,7 +1496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
@@ -1341,7 +1513,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>54</v>
       </c>
@@ -1359,7 +1531,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>54</v>
       </c>
@@ -1377,7 +1549,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>54</v>
       </c>
@@ -1395,7 +1567,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
@@ -1414,7 +1586,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>60</v>
       </c>
@@ -1432,20 +1604,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74E8795-B0D8-4BFA-BD93-DE9627104852}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.734375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1470,7 +1642,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1481,7 +1653,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1490,7 +1662,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1499,7 +1671,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1507,7 +1679,7 @@
         <v>-70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Add WIP receiver stuff
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcnelly/git-checkouts/adsbee/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA26E33-C806-474F-9C24-897554662671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E87E56-9115-8C4C-9FF9-6AB1D118324A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1280" windowWidth="24760" windowHeight="17460" firstSheet="3" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
+    <workbookView xWindow="-48180" yWindow="-16080" windowWidth="32300" windowHeight="23240" firstSheet="3" activeTab="3" xr2:uid="{ACA008B4-9B4D-4199-B30B-92BCAB53FB39}"/>
   </bookViews>
   <sheets>
     <sheet name="TLV3542 Noise Figure" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>Parameter</t>
   </si>
@@ -287,6 +287,9 @@
     <t>rssi_mid</t>
   </si>
   <si>
+    <t>rx_data_rate</t>
+  </si>
+  <si>
     <t>xosc_freq</t>
   </si>
   <si>
@@ -311,9 +314,6 @@
     <t>dwn2byp</t>
   </si>
   <si>
-    <t>sample_rate</t>
-  </si>
-  <si>
     <t>Sample rate for receiver I/Q and Bit Clock Recovery (BCR).</t>
   </si>
   <si>
@@ -326,7 +326,55 @@
     <t>12 bits, indicates 8x the desired oversampling rate.</t>
   </si>
   <si>
-    <t>rx_bit_rate</t>
+    <t>Stock WDS Value</t>
+  </si>
+  <si>
+    <t>ADSBee Value</t>
+  </si>
+  <si>
+    <t>2 bits</t>
+  </si>
+  <si>
+    <t>3 bits</t>
+  </si>
+  <si>
+    <t>ncoff</t>
+  </si>
+  <si>
+    <t>RX NCO accumulator overflow value multiplied by 64.</t>
+  </si>
+  <si>
+    <t>sampling_rate</t>
+  </si>
+  <si>
+    <t>1=Bypass an additional 3x decimator.</t>
+  </si>
+  <si>
+    <t>1=Bypass an additional 2x decimator.</t>
+  </si>
+  <si>
+    <t>bcr_sample_rate</t>
+  </si>
+  <si>
+    <t>Actual oversampling rate. Equal to bcr_sample_rate / rx_data_rate.</t>
+  </si>
+  <si>
+    <t>nco_offset</t>
+  </si>
+  <si>
+    <t>Sample rate of the bit clock recovery loop. Equal to the sampling rate divided by the rx oversampling rate.</t>
+  </si>
+  <si>
+    <t>Equal to the BCR sample rate divided by 8.</t>
+  </si>
+  <si>
+    <t>num_nco_offsets_per_overflow</t>
+  </si>
+  <si>
+    <t>How many NCO offset accumulates It takes to overflow the 22-bit register.</t>
+  </si>
+  <si>
+    <t>num_nco_overflows_per_second</t>
   </si>
 </sst>
 </file>
@@ -358,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +422,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -517,6 +571,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1331,126 +1387,247 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C90358F-5FC6-0B4A-A773-03445C27E3CB}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="46.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>30000000</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>30000000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <f>B2/2^B3/2^B4/2^B5/IF(B6,1,3)/IF(B7,1,2)/1000</f>
+        <v>30000</v>
+      </c>
+      <c r="C8">
+        <f>C2/2^C3/2^C4/2^C5/IF(C6,1,3)/IF(C7,1,2)/1000</f>
+        <v>30000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9">
-        <f>B2/B3/B4/B5/IF(B6,1,3)/IF(B7,1,2)/1000</f>
-        <v>250</v>
-      </c>
-      <c r="C9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
       <c r="B11">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>88</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="20">
         <f>B11/8</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7.5</v>
+      </c>
+      <c r="C12" s="20">
+        <f>C11/8</f>
+        <v>3.75</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B14">
-        <f>B9/B12</f>
-        <v>166.66666666666666</v>
+        <f>B8/B12</f>
+        <v>4000</v>
+      </c>
+      <c r="C14">
+        <f>C8/C12</f>
+        <v>8000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="6">
+        <f>B14/8</f>
+        <v>500</v>
+      </c>
+      <c r="C15" s="6">
+        <f>C14/8</f>
+        <v>1000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17">
+        <v>34953</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="21">
+        <f>B17/64</f>
+        <v>546.140625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="21">
+        <f>(2^22-1)/B18</f>
+        <v>7679.8956312762857</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20">
+        <f>B14/B19</f>
+        <v>0.52084041138658788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>